<commit_message>
Changed admob2.js to admob.js
</commit_message>
<xml_diff>
--- a/northern_colorado.xlsx
+++ b/northern_colorado.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="141">
   <si>
     <t>name</t>
   </si>
@@ -407,13 +407,92 @@
   </si>
   <si>
     <t>longitude</t>
+  </si>
+  <si>
+    <t>With a panoramic view of the scenic foothills of Fort Collins, Colorado, the brewery tour is an immersive experience where you can hear, smell, touch and taste the components that go into some of the world’s most popular beers.</t>
+  </si>
+  <si>
+    <t>We feature local Colorado grains in all of our beers from Troubadour Maltings in Fort Collins, allowing us to make a great product from local ingredients. Come find some of the best musical talent in our taproom and enjoy with a fresh beer made from the finest ingredients!</t>
+  </si>
+  <si>
+    <t>Since 2010, the Big Beaver Brewing Company has been creating delicious craft beer in the shadows of the Rocky Mountain National Park. This awe-inspiring view demands equally awesome beer, and the Big Beaver Brewery provides just that with 16 beers on tap to choose from. Enjoy your favorite beer in the cozy confines of our Taproom or to-go in refillable growlers. </t>
+  </si>
+  <si>
+    <t>Why Big Thompson Brewery? – It all started with the drive up the canyon and the gorgeous views of the powerful Big Thompson River.  It inspired our motto “Let The Beer Flow.”</t>
+  </si>
+  <si>
+    <t>Located in the heart of Midtown Fort Collins, CO. Black Bottle Brewery not only brews awesome craft beer in house, but we offer a full food menu through our brewpub. With 40 different beers on tap, we offer a wide selection of our own pride and joy, but don’t shy away from opening up our taps to our friends in the industry around the area or even around the world. Bringing in national favorites such as; Odell, Jolly Pumpkin, Sierra Nevada, and New Belgium, to name a few, our brewery has one of the widest selections of craft beer in Fort Collins as well as wine and a full bar. On top of that, you’ll often find a few taps pouring beers from international breweries as well.  In addition to those fine craft beers, our coolers are always stocked with a crazy good selection of bottled beers from all over the place. If you should you feel like kickin’ “it ol school,” you can even ask for that 40oz of OE (Old English) in a brown paper bag. We won’t judge. You won’t find a food truck here because we have a full restaurant to fill your plate.  Couple any of our beers with a full menu of gourmet food, not just beer nuts.  We’re the beer nuts</t>
+  </si>
+  <si>
+    <t>Not only do we offer the best selection of Colorado craft beer but we also brew in-house on our small batch three barrel system. Brix has been brewing tasteful beers thanks to long time Greeley resident &amp; brew master Jeremy Fusco. Fusco has established his brewing style by his culinary and German heritage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAND-CRAFTED MICRO BREWS DESIGNED FOR TASTE, SMOOTHNESS, AND QUALITY. Each of our beer recipes uses only the finest hops, wheat, barley, and other ingredients to combine for a fine tasting brew. The smoothness of each swallow is unsurpassed.  The beers you will enjoy are all within the traditional styles of craft beer with the occasional experimental batch thrown in. All of our beer is gluten reduced which does not change flavor or appearance! </t>
+  </si>
+  <si>
+    <t>We’re a four barrel nanobrewery with onsite sales and taproom. Craft brewing Colorado style, hands on and with help from our friends. We invite you to be part of the brewing experience!</t>
+  </si>
+  <si>
+    <t>We are dedicated to brewing high quality beer that we enjoy drinking, beer you can hang your hat on.</t>
+  </si>
+  <si>
+    <r>
+      <t>Naturally gluten-free </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF6A6A6A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>hard ciders</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF545454"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> made with 100% real fruit from a blend of tart and sweet </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF6A6A6A"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>apple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF545454"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>varieties. Light-bodied, effervescent, and refreshing.</t>
+    </r>
+  </si>
+  <si>
+    <t>See what's brewing at the CooperSmith's brewery, an important part of the Old Town Fort Collins culture. With over 147 different beers brewed since 1989, everyone will find something they love</t>
+  </si>
+  <si>
+    <t>Our mission is to build upon Fort Collins' excellent craft brewing heritage and apply these standards of quality to our distilling works. We produce premium, hand-crafted spirits that include vodka, whiskey, rum and liqueurs that will push your taste experience beyond mainstream, corporate producers</t>
+  </si>
+  <si>
+    <t>Weekly events, Brewery Tours, Seasonal Beers, Special Releases, Craft Soda, and an endless supply of super-cool people to talk to about beer and other important life issues currently gripping the nation. Crabtree Brewing Company is Greeley's destination brewery. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,6 +632,74 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF2F2E2E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF37280F"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF302222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Rubik"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Oswald"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFEFEFEF"/>
+      <name val="Open Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF545454"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF6A6A6A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF928372"/>
+      <name val="Proxima-nova"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Open Sans"/>
     </font>
   </fonts>
   <fills count="33">
@@ -896,10 +1043,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1221,19 +1379,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +1405,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1268,8 +1426,11 @@
         <f>CONCATENATE("&lt;option value=","""",C2,",",D2,""""," id=","""",A2,"""","&gt;",A2,"&lt;/option&gt;")</f>
         <v>&lt;option value="40.6202,-105.00594" id="Anheuser-Busch Inc - Fort Collins"&gt;Anheuser-Busch Inc - Fort Collins&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1290,8 +1451,11 @@
         <f t="shared" ref="F3:F63" si="1">CONCATENATE("&lt;option value=","""",C3,",",D3,""""," id=","""",A3,"""","&gt;",A3,"&lt;/option&gt;")</f>
         <v>&lt;option value="40.30443,-105.084847" id="Berthoud Brewing Company"&gt;Berthoud Brewing Company&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1312,8 +1476,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.40787,-105.11446" id="Big Beaver Brewing Co"&gt;Big Beaver Brewing Co&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1334,8 +1501,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.4078848,-105.0750355" id="Big Thompson Brewery"&gt;Big Thompson Brewery&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1356,8 +1526,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.56626,-105.07835" id="Black Bottle Brewery"&gt;Black Bottle Brewery&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1378,8 +1551,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.42517,-104.69161" id="Brix Taphouse and Brewery"&gt;Brix Taphouse and Brewery&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -1400,8 +1576,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.42198,-104.75734" id="Broken Plow Brewery"&gt;Broken Plow Brewery&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1422,8 +1601,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.40807,-105.13823" id="Buckhorn Brewers LLC"&gt;Buckhorn Brewers LLC&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1444,8 +1626,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.30489,-105.07897" id="City Star Brewing"&gt;City Star Brewing&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G10" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -1466,8 +1651,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.40787,-105.11446" id="Climb Hard Cider Co"&gt;Climb Hard Cider Co&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1488,8 +1676,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.58737,-105.07582" id="CooperSmiths Pub and Brewing"&gt;CooperSmiths Pub and Brewing&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G12" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1510,8 +1701,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.5901,-105.07651" id="Coppermuse Distillery"&gt;Coppermuse Distillery&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="23.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1532,8 +1726,11 @@
         <f t="shared" si="1"/>
         <v>&lt;option value="40.39107,-104.72674" id="Crabtree Brewing"&gt;Crabtree Brewing&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G14" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1555,7 +1752,7 @@
         <v>&lt;option value="40.58976,-105.07649" id="Crooked Stave Artisan Beer Project"&gt;Crooked Stave Artisan Beer Project&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1577,7 +1774,7 @@
         <v>&lt;option value="40.391524,-105.0597283" id="Crow Hop Brewing Co. Ltd."&gt;Crow Hop Brewing Co. Ltd.&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1599,7 +1796,7 @@
         <v>&lt;option value="40.5231471,-105.0210651" id="D.C. Oakes Brewhouse and Eatery"&gt;D.C. Oakes Brewhouse and Eatery&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1621,7 +1818,7 @@
         <v>&lt;option value="40.403188,-105.0678394" id="Dratz Brewing Company"&gt;Dratz Brewing Company&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75">
       <c r="A19" t="s">
         <v>56</v>
       </c>
@@ -1643,7 +1840,7 @@
         <v>&lt;option value="40.55178,-105.05838" id="Elevations 5003"&gt;Elevations 5003&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1665,7 +1862,7 @@
         <v>&lt;option value="40.58625,-105.07585" id="Equinox Brewing"&gt;Equinox Brewing&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -1687,7 +1884,7 @@
         <v>&lt;option value="40.58472,-105.04596" id="Feisty Spirits"&gt;Feisty Spirits&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +1906,7 @@
         <v>&lt;option value="40.58344,-105.04338" id="Funkwerks"&gt;Funkwerks&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1731,7 +1928,7 @@
         <v>&lt;option value="40.52231,-104.85583" id="G5 Brewpub"&gt;G5 Brewpub&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1753,7 +1950,7 @@
         <v>&lt;option value="40.53937,-105.07532" id="Gilded Goat Brewing Company"&gt;Gilded Goat Brewing Company&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1775,7 +1972,7 @@
         <v>&lt;option value="40.42279,-104.69024" id="Green Earth Brewing Company"&gt;Green Earth Brewing Company&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1797,7 +1994,7 @@
         <v>&lt;option value="40.39776,-105.04486" id="Grimm Brothers Brewhouse, LLC"&gt;Grimm Brothers Brewhouse, LLC&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1819,7 +2016,7 @@
         <v>&lt;option value="40.48088,-104.9361" id="High Hops Brewery"&gt;High Hops Brewery&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1841,7 +2038,7 @@
         <v>&lt;option value="40.58965,-105.04562" id="Horse &amp; Dragon Brewing Company"&gt;Horse &amp; Dragon Brewing Company&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>125</v>
       </c>
@@ -1863,7 +2060,7 @@
         <v>&lt;option value="40.52495,-104.85663" id="Hunters Moon Meadery"&gt;Hunters Moon Meadery&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1885,7 +2082,7 @@
         <v>&lt;option value="40.58976,-105.07649" id="Infinite Monkey Theorem"&gt;Infinite Monkey Theorem&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1907,7 +2104,7 @@
         <v>&lt;option value="40.55297,-105.1162" id="Intersect Brewing"&gt;Intersect Brewing&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1929,7 +2126,7 @@
         <v>&lt;option value="40.56219,-105.037862" id="Jessup Farm Barrel House"&gt;Jessup Farm Barrel House&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1951,7 +2148,7 @@
         <v>&lt;option value="40.3953482,-105.0773757" id="Loveland Aleworks"&gt;Loveland Aleworks&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -1973,7 +2170,7 @@
         <v>&lt;option value="40.43786,-104.9682" id="Mash Lab Brewing"&gt;Mash Lab Brewing&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -1995,7 +2192,7 @@
         <v>&lt;option value="40.54985,-105.07937" id="Maxline Brewing"&gt;Maxline Brewing&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2017,7 +2214,7 @@
         <v>&lt;option value="40.57292,-105.11541" id="McClellan's Brewing Company"&gt;McClellan's Brewing Company&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -2039,7 +2236,7 @@
         <v>&lt;option value="40.4573036,-104.9828003" id="Mighty River Brewing Company"&gt;Mighty River Brewing Company&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.75">
       <c r="A38" t="s">
         <v>58</v>
       </c>
@@ -2061,7 +2258,7 @@
         <v>&lt;option value="40.59012,-105.07236" id="Mobb Mountain Distillery"&gt;Mobb Mountain Distillery&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>15</v>
       </c>
@@ -2083,7 +2280,7 @@
         <v>&lt;option value="40.59341,-105.06687" id="New Belgium Brewing Co"&gt;New Belgium Brewing Co&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15.75">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -2105,7 +2302,7 @@
         <v>&lt;option value="40.58358,-105.04801" id="NOCO Distillery"&gt;NOCO Distillery&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -2127,7 +2324,7 @@
         <v>&lt;option value="40.5889,-105.06025" id="Odell Brewing Co"&gt;Odell Brewing Co&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15.75">
       <c r="A42" t="s">
         <v>59</v>
       </c>
@@ -2149,7 +2346,7 @@
         <v>&lt;option value="40.59132,-105.05052" id="Old Town Distilling Co"&gt;Old Town Distilling Co&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15.75">
       <c r="A43" t="s">
         <v>17</v>
       </c>
@@ -2171,7 +2368,7 @@
         <v>&lt;option value="40.5884014,-105.074634" id="Prost Brewing Fort Collins"&gt;Prost Brewing Fort Collins&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -2193,7 +2390,7 @@
         <v>&lt;option value="40.53116,-105.08009" id="Purpose Brewing and Cellars"&gt;Purpose Brewing and Cellars&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>19</v>
       </c>
@@ -2215,7 +2412,7 @@
         <v>&lt;option value="40.5666,-105.05774" id="Rally King Brewing"&gt;Rally King Brewing&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -2237,7 +2434,7 @@
         <v>&lt;option value="40.5779533,-105.080925" id="Ramskeller"&gt;Ramskeller&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -2259,7 +2456,7 @@
         <v>&lt;option value="40.58926,-105.05852" id="Red Truck Beer Company Ltd."&gt;Red Truck Beer Company Ltd.&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -2281,7 +2478,7 @@
         <v>&lt;option value="40.418352,-104.9904337" id="Rock Bottom Brewery - Centerra Promenade"&gt;Rock Bottom Brewery - Centerra Promenade&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -2303,7 +2500,7 @@
         <v>&lt;option value="40.39721,-105.0713" id="Rock Coast Brewery"&gt;Rock Coast Brewery&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -2325,7 +2522,7 @@
         <v>&lt;option value="40.38786,-104.78599" id="Rocky Mountain Taphouse, LLC"&gt;Rocky Mountain Taphouse, LLC&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15.75">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -2347,7 +2544,7 @@
         <v>&lt;option value="40.58949,-105.07749" id="Scrumpys"&gt;Scrumpys&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>22</v>
       </c>
@@ -2369,7 +2566,7 @@
         <v>&lt;option value="40.58993,-105.05872" id="Snowbank Brewing"&gt;Snowbank Brewing&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -2391,7 +2588,7 @@
         <v>&lt;option value="40.6770298,-105.0690762" id="Soul Squared Brewing Co."&gt;Soul Squared Brewing Co.&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15.75">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -2413,7 +2610,7 @@
         <v>&lt;option value="40.46004,-105.08296" id="Spring 44 Distilling"&gt;Spring 44 Distilling&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15.75">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -2435,7 +2632,7 @@
         <v>&lt;option value="40.40758,-105.1578" id="Sweet Heart Winery"&gt;Sweet Heart Winery&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15.75">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2457,7 +2654,7 @@
         <v>&lt;option value="40.6533187,-105.169607" id="Ten Bears Winery"&gt;Ten Bears Winery&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>46</v>
       </c>
@@ -2479,7 +2676,7 @@
         <v>&lt;option value="40.4209055,-105.07711" id="Tilted Barrel Brew Pub"&gt;Tilted Barrel Brew Pub&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -2501,7 +2698,7 @@
         <v>&lt;option value="40.5080757,-104.9560623" id="Timnath Beerwerks"&gt;Timnath Beerwerks&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -2523,7 +2720,7 @@
         <v>&lt;option value="40.39681,-105.07511" id="Verboten Brewing"&gt;Verboten Brewing&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -2545,7 +2742,7 @@
         <v>&lt;option value="40.33684,-104.90583" id="Veteran Brothers Brewing Company"&gt;Veteran Brothers Brewing Company&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>50</v>
       </c>
@@ -2567,7 +2764,7 @@
         <v>&lt;option value="40.42782,-104.68997" id="WeldWerks Brewing Co."&gt;WeldWerks Brewing Co.&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>51</v>
       </c>
@@ -2589,7 +2786,7 @@
         <v>&lt;option value="40.43196,-104.68852" id="Wiley Roots Brewing Co"&gt;Wiley Roots Brewing Co&lt;/option&gt;</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>24</v>
       </c>

</xml_diff>